<commit_message>
Right now I am looking to normalize and plot these data with significance markers
</commit_message>
<xml_diff>
--- a/Data/data_master.xlsx
+++ b/Data/data_master.xlsx
@@ -1,24 +1,83 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MicrobeJ\Documents\R_projects\with_trainees\PhiCB5-AbsorptionAssay\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B57831-8EF9-4445-93CC-DDCEF1EC4A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27420" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="16">
+  <si>
+    <t>strain</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>rep</t>
+  </si>
+  <si>
+    <t>titer</t>
+  </si>
+  <si>
+    <t>genotype</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>LZ22208</t>
+  </si>
+  <si>
+    <t>NA1000</t>
+  </si>
+  <si>
+    <t>LZ22209</t>
+  </si>
+  <si>
+    <t>NA1000 ▲pilA</t>
+  </si>
+  <si>
+    <t>negative control</t>
+  </si>
+  <si>
+    <t>No Cell Control</t>
+  </si>
+  <si>
+    <t>LZ22221</t>
+  </si>
+  <si>
+    <t>bNY30a</t>
+  </si>
+  <si>
+    <t>LZ22223</t>
+  </si>
+  <si>
+    <t>pilAT36C</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd HH:mm:ss UTC"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss\ \U\T\C"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,13 +126,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -111,7 +178,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -145,6 +212,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -179,9 +247,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -354,53 +423,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F69"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>strain</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>rep</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>titer</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>genotype</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>n</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
       </c>
       <c r="B2" s="2">
         <v>44965</v>
@@ -411,20 +468,16 @@
       <c r="D2">
         <v>165</v>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E2" t="s">
+        <v>7</v>
       </c>
       <c r="F2">
         <v>12</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
       </c>
       <c r="B3" s="2">
         <v>44965</v>
@@ -435,20 +488,16 @@
       <c r="D3">
         <v>158</v>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
       <c r="F3">
         <v>12</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>44965</v>
@@ -459,20 +508,16 @@
       <c r="D4">
         <v>231</v>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
       <c r="F4">
         <v>24</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
       </c>
       <c r="B5" s="2">
         <v>44965</v>
@@ -483,20 +528,16 @@
       <c r="D5">
         <v>92</v>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E5" t="s">
+        <v>13</v>
       </c>
       <c r="F5">
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>44970</v>
@@ -507,20 +548,16 @@
       <c r="D6">
         <v>191</v>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E6" t="s">
+        <v>7</v>
       </c>
       <c r="F6">
         <v>12</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>44970</v>
@@ -531,20 +568,16 @@
       <c r="D7">
         <v>190</v>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
       <c r="F7">
         <v>12</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
       </c>
       <c r="B8" s="2">
         <v>44970</v>
@@ -555,20 +588,16 @@
       <c r="D8">
         <v>100</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E8" t="s">
+        <v>13</v>
       </c>
       <c r="F8">
         <v>11</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="2">
         <v>44970</v>
@@ -579,20 +608,16 @@
       <c r="D9">
         <v>198</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E9" t="s">
+        <v>11</v>
       </c>
       <c r="F9">
         <v>24</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
       </c>
       <c r="B10" s="2">
         <v>44970</v>
@@ -603,20 +628,16 @@
       <c r="D10">
         <v>310</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E10" t="s">
+        <v>7</v>
       </c>
       <c r="F10">
         <v>12</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
       </c>
       <c r="B11" s="2">
         <v>44970</v>
@@ -627,20 +648,16 @@
       <c r="D11">
         <v>291</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E11" t="s">
+        <v>9</v>
       </c>
       <c r="F11">
         <v>12</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
       </c>
       <c r="B12" s="2">
         <v>44970</v>
@@ -651,20 +668,16 @@
       <c r="D12">
         <v>160</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E12" t="s">
+        <v>13</v>
       </c>
       <c r="F12">
         <v>11</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
       </c>
       <c r="B13" s="2">
         <v>44970</v>
@@ -675,20 +688,16 @@
       <c r="D13">
         <v>298</v>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E13" t="s">
+        <v>11</v>
       </c>
       <c r="F13">
         <v>24</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
       </c>
       <c r="B14" s="2">
         <v>44970</v>
@@ -699,20 +708,16 @@
       <c r="D14">
         <v>125</v>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E14" t="s">
+        <v>7</v>
       </c>
       <c r="F14">
         <v>12</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>8</v>
       </c>
       <c r="B15" s="2">
         <v>44970</v>
@@ -723,20 +728,16 @@
       <c r="D15">
         <v>137</v>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E15" t="s">
+        <v>9</v>
       </c>
       <c r="F15">
         <v>12</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
       </c>
       <c r="B16" s="2">
         <v>44970</v>
@@ -747,20 +748,16 @@
       <c r="D16">
         <v>68</v>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E16" t="s">
+        <v>13</v>
       </c>
       <c r="F16">
         <v>11</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>10</v>
       </c>
       <c r="B17" s="2">
         <v>44970</v>
@@ -771,20 +768,16 @@
       <c r="D17">
         <v>145</v>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E17" t="s">
+        <v>11</v>
       </c>
       <c r="F17">
         <v>24</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
       </c>
       <c r="B18" s="2">
         <v>44965</v>
@@ -795,20 +788,16 @@
       <c r="D18">
         <v>140</v>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E18" t="s">
+        <v>7</v>
       </c>
       <c r="F18">
         <v>12</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>8</v>
       </c>
       <c r="B19" s="2">
         <v>44965</v>
@@ -819,20 +808,16 @@
       <c r="D19">
         <v>120</v>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E19" t="s">
+        <v>9</v>
       </c>
       <c r="F19">
         <v>12</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
       </c>
       <c r="B20" s="2">
         <v>44965</v>
@@ -843,20 +828,16 @@
       <c r="D20">
         <v>82</v>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E20" t="s">
+        <v>13</v>
       </c>
       <c r="F20">
         <v>11</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>10</v>
       </c>
       <c r="B21" s="2">
         <v>44965</v>
@@ -867,20 +848,16 @@
       <c r="D21">
         <v>229</v>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E21" t="s">
+        <v>11</v>
       </c>
       <c r="F21">
         <v>24</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
       </c>
       <c r="B22" s="2">
         <v>44970</v>
@@ -891,20 +868,16 @@
       <c r="D22">
         <v>172</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E22" t="s">
+        <v>7</v>
       </c>
       <c r="F22">
         <v>12</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>8</v>
       </c>
       <c r="B23" s="2">
         <v>44970</v>
@@ -915,20 +888,16 @@
       <c r="D23">
         <v>198</v>
       </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E23" t="s">
+        <v>9</v>
       </c>
       <c r="F23">
         <v>12</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>12</v>
       </c>
       <c r="B24" s="2">
         <v>44970</v>
@@ -939,20 +908,16 @@
       <c r="D24">
         <v>126</v>
       </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E24" t="s">
+        <v>13</v>
       </c>
       <c r="F24">
         <v>11</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>10</v>
       </c>
       <c r="B25" s="2">
         <v>44970</v>
@@ -963,20 +928,16 @@
       <c r="D25">
         <v>196</v>
       </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E25" t="s">
+        <v>11</v>
       </c>
       <c r="F25">
         <v>24</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
       </c>
       <c r="B26" s="2">
         <v>44970</v>
@@ -987,20 +948,16 @@
       <c r="D26">
         <v>299</v>
       </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E26" t="s">
+        <v>7</v>
       </c>
       <c r="F26">
         <v>12</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>8</v>
       </c>
       <c r="B27" s="2">
         <v>44970</v>
@@ -1011,20 +968,16 @@
       <c r="D27">
         <v>318</v>
       </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E27" t="s">
+        <v>9</v>
       </c>
       <c r="F27">
         <v>12</v>
       </c>
     </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>12</v>
       </c>
       <c r="B28" s="2">
         <v>44970</v>
@@ -1035,20 +988,16 @@
       <c r="D28">
         <v>181</v>
       </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E28" t="s">
+        <v>13</v>
       </c>
       <c r="F28">
         <v>11</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
       </c>
       <c r="B29" s="2">
         <v>44970</v>
@@ -1059,20 +1008,16 @@
       <c r="D29">
         <v>298</v>
       </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E29" t="s">
+        <v>11</v>
       </c>
       <c r="F29">
         <v>24</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>6</v>
       </c>
       <c r="B30" s="2">
         <v>44970</v>
@@ -1083,20 +1028,16 @@
       <c r="D30">
         <v>124</v>
       </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E30" t="s">
+        <v>7</v>
       </c>
       <c r="F30">
         <v>12</v>
       </c>
     </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
       </c>
       <c r="B31" s="2">
         <v>44970</v>
@@ -1107,20 +1048,16 @@
       <c r="D31">
         <v>130</v>
       </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E31" t="s">
+        <v>9</v>
       </c>
       <c r="F31">
         <v>12</v>
       </c>
     </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>12</v>
       </c>
       <c r="B32" s="2">
         <v>44970</v>
@@ -1131,20 +1068,16 @@
       <c r="D32">
         <v>75</v>
       </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E32" t="s">
+        <v>13</v>
       </c>
       <c r="F32">
         <v>11</v>
       </c>
     </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>10</v>
       </c>
       <c r="B33" s="2">
         <v>44970</v>
@@ -1155,20 +1088,16 @@
       <c r="D33">
         <v>142</v>
       </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E33" t="s">
+        <v>11</v>
       </c>
       <c r="F33">
         <v>24</v>
       </c>
     </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>6</v>
       </c>
       <c r="B34" s="2">
         <v>44965</v>
@@ -1179,20 +1108,16 @@
       <c r="D34">
         <v>178</v>
       </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E34" t="s">
+        <v>7</v>
       </c>
       <c r="F34">
         <v>12</v>
       </c>
     </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>8</v>
       </c>
       <c r="B35" s="2">
         <v>44965</v>
@@ -1203,20 +1128,16 @@
       <c r="D35">
         <v>187</v>
       </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E35" t="s">
+        <v>9</v>
       </c>
       <c r="F35">
         <v>12</v>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>12</v>
       </c>
       <c r="B36" s="2">
         <v>44965</v>
@@ -1227,20 +1148,16 @@
       <c r="D36">
         <v>76</v>
       </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E36" t="s">
+        <v>13</v>
       </c>
       <c r="F36">
         <v>11</v>
       </c>
     </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>10</v>
       </c>
       <c r="B37" s="2">
         <v>44965</v>
@@ -1251,20 +1168,16 @@
       <c r="D37">
         <v>218</v>
       </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E37" t="s">
+        <v>11</v>
       </c>
       <c r="F37">
         <v>24</v>
       </c>
     </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>6</v>
       </c>
       <c r="B38" s="2">
         <v>44970</v>
@@ -1275,20 +1188,16 @@
       <c r="D38">
         <v>166</v>
       </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E38" t="s">
+        <v>7</v>
       </c>
       <c r="F38">
         <v>12</v>
       </c>
     </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>8</v>
       </c>
       <c r="B39" s="2">
         <v>44970</v>
@@ -1299,20 +1208,16 @@
       <c r="D39">
         <v>195</v>
       </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E39" t="s">
+        <v>9</v>
       </c>
       <c r="F39">
         <v>12</v>
       </c>
     </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>12</v>
       </c>
       <c r="B40" s="2">
         <v>44970</v>
@@ -1323,20 +1228,16 @@
       <c r="D40">
         <v>125</v>
       </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E40" t="s">
+        <v>13</v>
       </c>
       <c r="F40">
         <v>11</v>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>10</v>
       </c>
       <c r="B41" s="2">
         <v>44970</v>
@@ -1347,20 +1248,16 @@
       <c r="D41">
         <v>192</v>
       </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E41" t="s">
+        <v>11</v>
       </c>
       <c r="F41">
         <v>24</v>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>6</v>
       </c>
       <c r="B42" s="2">
         <v>44970</v>
@@ -1371,20 +1268,16 @@
       <c r="D42">
         <v>296</v>
       </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E42" t="s">
+        <v>7</v>
       </c>
       <c r="F42">
         <v>12</v>
       </c>
     </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>8</v>
       </c>
       <c r="B43" s="2">
         <v>44970</v>
@@ -1395,20 +1288,16 @@
       <c r="D43">
         <v>308</v>
       </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E43" t="s">
+        <v>9</v>
       </c>
       <c r="F43">
         <v>12</v>
       </c>
     </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>LZ22221</t>
-        </is>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>12</v>
       </c>
       <c r="B44" s="2">
         <v>44970</v>
@@ -1419,20 +1308,16 @@
       <c r="D44">
         <v>178</v>
       </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>bNY30a</t>
-        </is>
+      <c r="E44" t="s">
+        <v>13</v>
       </c>
       <c r="F44">
         <v>11</v>
       </c>
     </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>10</v>
       </c>
       <c r="B45" s="2">
         <v>44970</v>
@@ -1443,20 +1328,16 @@
       <c r="D45">
         <v>294</v>
       </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E45" t="s">
+        <v>11</v>
       </c>
       <c r="F45">
         <v>24</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>LZ22208</t>
-        </is>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>6</v>
       </c>
       <c r="B46" s="2">
         <v>44970</v>
@@ -1467,20 +1348,16 @@
       <c r="D46">
         <v>125</v>
       </c>
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>NA1000</t>
-        </is>
+      <c r="E46" t="s">
+        <v>7</v>
       </c>
       <c r="F46">
         <v>12</v>
       </c>
     </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>LZ22209</t>
-        </is>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>8</v>
       </c>
       <c r="B47" s="2">
         <v>44970</v>
@@ -1491,20 +1368,16 @@
       <c r="D47">
         <v>131</v>
       </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>NA1000 ▲pilA</t>
-        </is>
+      <c r="E47" t="s">
+        <v>9</v>
       </c>
       <c r="F47">
         <v>12</v>
       </c>
     </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>10</v>
       </c>
       <c r="B48" s="2">
         <v>44970</v>
@@ -1515,20 +1388,16 @@
       <c r="D48">
         <v>144</v>
       </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E48" t="s">
+        <v>11</v>
       </c>
       <c r="F48">
         <v>24</v>
       </c>
     </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>14</v>
       </c>
       <c r="B49" s="2">
         <v>45178</v>
@@ -1539,20 +1408,16 @@
       <c r="D49">
         <v>115</v>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E49" t="s">
+        <v>15</v>
       </c>
       <c r="F49">
         <v>9</v>
       </c>
     </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>14</v>
       </c>
       <c r="B50" s="2">
         <v>45178</v>
@@ -1563,20 +1428,16 @@
       <c r="D50">
         <v>85</v>
       </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E50" t="s">
+        <v>15</v>
       </c>
       <c r="F50">
         <v>9</v>
       </c>
     </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>14</v>
       </c>
       <c r="B51" s="2">
         <v>45178</v>
@@ -1587,20 +1448,16 @@
       <c r="D51">
         <v>122</v>
       </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E51" t="s">
+        <v>15</v>
       </c>
       <c r="F51">
         <v>9</v>
       </c>
     </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>14</v>
       </c>
       <c r="B52" s="2">
         <v>45179</v>
@@ -1611,20 +1468,16 @@
       <c r="D52">
         <v>162</v>
       </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E52" t="s">
+        <v>15</v>
       </c>
       <c r="F52">
         <v>9</v>
       </c>
     </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>14</v>
       </c>
       <c r="B53" s="2">
         <v>45179</v>
@@ -1635,20 +1488,16 @@
       <c r="D53">
         <v>81</v>
       </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E53" t="s">
+        <v>15</v>
       </c>
       <c r="F53">
         <v>9</v>
       </c>
     </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>14</v>
       </c>
       <c r="B54" s="2">
         <v>45179</v>
@@ -1659,20 +1508,16 @@
       <c r="D54">
         <v>81</v>
       </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E54" t="s">
+        <v>15</v>
       </c>
       <c r="F54">
         <v>9</v>
       </c>
     </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>14</v>
       </c>
       <c r="B55" s="2">
         <v>45181</v>
@@ -1683,20 +1528,16 @@
       <c r="D55">
         <v>165</v>
       </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E55" t="s">
+        <v>15</v>
       </c>
       <c r="F55">
         <v>9</v>
       </c>
     </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>14</v>
       </c>
       <c r="B56" s="2">
         <v>45181</v>
@@ -1707,20 +1548,16 @@
       <c r="D56">
         <v>127</v>
       </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E56" t="s">
+        <v>15</v>
       </c>
       <c r="F56">
         <v>9</v>
       </c>
     </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>LZ22223</t>
-        </is>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>14</v>
       </c>
       <c r="B57" s="2">
         <v>45181</v>
@@ -1731,300 +1568,190 @@
       <c r="D57">
         <v>70</v>
       </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>pilAT36C</t>
-        </is>
+      <c r="E57" t="s">
+        <v>15</v>
       </c>
       <c r="F57">
         <v>9</v>
       </c>
     </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>10</v>
       </c>
       <c r="B58" s="2">
-        <v>45177</v>
+        <v>45178</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58">
-        <v>222</v>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+        <v>254</v>
+      </c>
+      <c r="E58" t="s">
+        <v>11</v>
       </c>
       <c r="F58">
         <v>24</v>
       </c>
     </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>10</v>
       </c>
       <c r="B59" s="2">
-        <v>45177</v>
+        <v>45178</v>
       </c>
       <c r="C59">
         <v>2</v>
       </c>
       <c r="D59">
+        <v>218</v>
+      </c>
+      <c r="E59" t="s">
+        <v>11</v>
+      </c>
+      <c r="F59">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>10</v>
+      </c>
+      <c r="B60" s="2">
+        <v>45178</v>
+      </c>
+      <c r="C60">
+        <v>3</v>
+      </c>
+      <c r="D60">
+        <v>223</v>
+      </c>
+      <c r="E60" t="s">
+        <v>11</v>
+      </c>
+      <c r="F60">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>10</v>
+      </c>
+      <c r="B61" s="2">
+        <v>45179</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>307</v>
+      </c>
+      <c r="E61" t="s">
+        <v>11</v>
+      </c>
+      <c r="F61">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>10</v>
+      </c>
+      <c r="B62" s="2">
+        <v>45179</v>
+      </c>
+      <c r="C62">
+        <v>2</v>
+      </c>
+      <c r="D62">
+        <v>267</v>
+      </c>
+      <c r="E62" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="2">
+        <v>45179</v>
+      </c>
+      <c r="C63">
+        <v>3</v>
+      </c>
+      <c r="D63">
         <v>207</v>
       </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
-      </c>
-      <c r="F59">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
-      </c>
-      <c r="B60" s="2">
-        <v>45177</v>
-      </c>
-      <c r="C60">
-        <v>3</v>
-      </c>
-      <c r="D60">
-        <v>226</v>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
-      </c>
-      <c r="F60">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
-      </c>
-      <c r="B61" s="2">
-        <v>45178</v>
-      </c>
-      <c r="C61">
-        <v>1</v>
-      </c>
-      <c r="D61">
-        <v>254</v>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
-      </c>
-      <c r="F61">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
-      </c>
-      <c r="B62" s="2">
-        <v>45178</v>
-      </c>
-      <c r="C62">
-        <v>2</v>
-      </c>
-      <c r="D62">
-        <v>218</v>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
-      </c>
-      <c r="F62">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
-      </c>
-      <c r="B63" s="2">
-        <v>45178</v>
-      </c>
-      <c r="C63">
-        <v>3</v>
-      </c>
-      <c r="D63">
-        <v>223</v>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+      <c r="E63" t="s">
+        <v>11</v>
       </c>
       <c r="F63">
         <v>24</v>
       </c>
     </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>10</v>
       </c>
       <c r="B64" s="2">
-        <v>45179</v>
+        <v>45181</v>
       </c>
       <c r="C64">
         <v>1</v>
       </c>
       <c r="D64">
-        <v>307</v>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+        <v>248</v>
+      </c>
+      <c r="E64" t="s">
+        <v>11</v>
       </c>
       <c r="F64">
         <v>24</v>
       </c>
     </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>10</v>
       </c>
       <c r="B65" s="2">
-        <v>45179</v>
+        <v>45181</v>
       </c>
       <c r="C65">
         <v>2</v>
       </c>
       <c r="D65">
-        <v>267</v>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+        <v>209</v>
+      </c>
+      <c r="E65" t="s">
+        <v>11</v>
       </c>
       <c r="F65">
         <v>24</v>
       </c>
     </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>10</v>
       </c>
       <c r="B66" s="2">
-        <v>45179</v>
+        <v>45181</v>
       </c>
       <c r="C66">
         <v>3</v>
       </c>
       <c r="D66">
-        <v>207</v>
-      </c>
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
+        <v>211</v>
+      </c>
+      <c r="E66" t="s">
+        <v>11</v>
       </c>
       <c r="F66">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
-      </c>
-      <c r="B67" s="2">
-        <v>45181</v>
-      </c>
-      <c r="C67">
-        <v>1</v>
-      </c>
-      <c r="D67">
-        <v>248</v>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
-      </c>
-      <c r="F67">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
-      </c>
-      <c r="B68" s="2">
-        <v>45181</v>
-      </c>
-      <c r="C68">
-        <v>2</v>
-      </c>
-      <c r="D68">
-        <v>209</v>
-      </c>
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
-      </c>
-      <c r="F68">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>negative control</t>
-        </is>
-      </c>
-      <c r="B69" s="2">
-        <v>45181</v>
-      </c>
-      <c r="C69">
-        <v>3</v>
-      </c>
-      <c r="D69">
-        <v>211</v>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>No Cell Control</t>
-        </is>
-      </c>
-      <c r="F69">
         <v>24</v>
       </c>
     </row>

</xml_diff>